<commit_message>
Finalized Budget Reconciliation Page!
</commit_message>
<xml_diff>
--- a/test_files/FY 25 Foundation Summary Tester copy.xlsx
+++ b/test_files/FY 25 Foundation Summary Tester copy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinsabbe/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinsabbe/Documents/Sports Programs/Player Eligibility Flask/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CC12D5-A8F8-494F-A699-39F905DCBFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5412BA46-788C-194C-88B8-C644B01A1F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" tabRatio="838" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,9 +173,6 @@
     <t xml:space="preserve">15490 Oakdale Rd. Dallas OR 97338-9107 </t>
   </si>
   <si>
-    <t xml:space="preserve">Hunter-Jumper </t>
-  </si>
-  <si>
     <t>FY19 Beginning Balance</t>
   </si>
   <si>
@@ -341,12 +338,6 @@
     <t>Men's Water Polo</t>
   </si>
   <si>
-    <t>Polo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OSU Tennis </t>
-  </si>
-  <si>
     <t xml:space="preserve">Racquetball </t>
   </si>
   <si>
@@ -374,10 +365,19 @@
     <t xml:space="preserve">Triathlon </t>
   </si>
   <si>
-    <t>Bass Fishing</t>
-  </si>
-  <si>
     <t>Sports Clubs</t>
+  </si>
+  <si>
+    <t>Equestrian Polo</t>
+  </si>
+  <si>
+    <t>Fishing</t>
+  </si>
+  <si>
+    <t>Marksmanship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equestrian Hunter-Jumper </t>
   </si>
 </sst>
 </file>
@@ -2017,7 +2017,7 @@
     <row r="2" spans="2:8" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="12">
         <v>12391.71</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="14">
         <f>C3+C4-C5</f>
@@ -2086,13 +2086,13 @@
         <v>43369</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="6">
         <v>100</v>
@@ -2110,13 +2110,13 @@
         <v>43377</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" s="6">
         <v>50</v>
@@ -2133,13 +2133,13 @@
         <v>43383</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" s="6">
         <v>50</v>
@@ -2156,13 +2156,13 @@
         <v>43448</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="F12" s="6">
         <v>284.08</v>
@@ -2180,13 +2180,13 @@
         <v>43462</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="33" t="s">
         <v>78</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>79</v>
       </c>
       <c r="F13" s="6">
         <v>400</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="12">
         <v>3331.7</v>
@@ -2281,7 +2281,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="14">
         <f>C3+C4-C5</f>
@@ -2359,7 +2359,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="12">
         <v>1726.35</v>
@@ -2385,7 +2385,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="14">
         <f>C3+C4-C5</f>
@@ -2421,13 +2421,13 @@
         <v>43487</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="F9" s="6">
         <v>25</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="12">
         <v>2351.6799999999998</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="14">
         <f>C3+C4-C5</f>
@@ -2547,7 +2547,7 @@
         <v>43373</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="6">
         <v>238.92</v>
@@ -2561,7 +2561,7 @@
         <v>43465</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="6">
         <v>241.64</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="12">
         <v>6005.64</v>
@@ -2650,7 +2650,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="14">
         <f>C2+C3-C4</f>
@@ -2689,7 +2689,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="6">
         <v>50</v>
@@ -2732,7 +2732,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="6">
         <v>50</v>
@@ -2775,7 +2775,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="6">
         <v>50</v>
@@ -2817,7 +2817,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="6">
         <v>25</v>
@@ -2828,7 +2828,7 @@
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
@@ -2839,7 +2839,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="6">
         <v>25</v>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="G15" s="26"/>
       <c r="H15" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="16" x14ac:dyDescent="0.2">
@@ -2861,7 +2861,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="6">
         <v>25</v>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="G16" s="26"/>
       <c r="H16" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
@@ -2883,7 +2883,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17" s="6">
         <v>50</v>
@@ -2894,7 +2894,7 @@
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
@@ -2905,7 +2905,7 @@
         <v>14</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" s="6">
         <v>50</v>
@@ -2927,7 +2927,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="6">
         <v>45</v>
@@ -2948,7 +2948,7 @@
         <v>14</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E20" s="6">
         <v>32</v>
@@ -2958,7 +2958,7 @@
       </c>
       <c r="G20" s="26"/>
       <c r="H20" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
@@ -2969,7 +2969,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="6">
         <v>50</v>
@@ -2991,7 +2991,7 @@
         <v>14</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E22" s="6">
         <v>45</v>
@@ -3012,7 +3012,7 @@
         <v>14</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23" s="6">
         <v>45</v>
@@ -3033,7 +3033,7 @@
         <v>14</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E24" s="6">
         <v>500</v>
@@ -3054,7 +3054,7 @@
         <v>14</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="6">
         <v>50</v>
@@ -3076,7 +3076,7 @@
         <v>14</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E26" s="6">
         <v>45</v>
@@ -3097,7 +3097,7 @@
         <v>14</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E27" s="23">
         <v>50</v>
@@ -3115,10 +3115,10 @@
         <v>43327</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E28" s="6"/>
       <c r="G28" s="26">
@@ -3131,10 +3131,10 @@
         <v>43391</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="E29" s="6"/>
       <c r="G29" s="26">
@@ -3147,10 +3147,10 @@
         <v>43444</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="6"/>
       <c r="G30" s="26">
@@ -3193,7 +3193,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3207,10 +3207,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>18</v>
@@ -3227,7 +3227,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="39">
         <v>1299.04</v>
@@ -3242,7 +3242,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="54">
         <v>0</v>
@@ -3257,7 +3257,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="42">
         <v>8736.52</v>
@@ -3272,7 +3272,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="42">
         <v>95.36</v>
@@ -3287,7 +3287,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="42">
         <v>2730.62</v>
@@ -3332,7 +3332,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="42">
         <v>984.69999999999993</v>
@@ -3362,7 +3362,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="42">
         <v>1043.8499999999999</v>
@@ -3377,47 +3377,47 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B12" s="42">
-        <v>475</v>
+        <v>425.35</v>
       </c>
       <c r="C12" s="42"/>
       <c r="D12" s="43"/>
       <c r="E12" s="43"/>
       <c r="F12" s="44">
         <f>B12+C12-D12-E12</f>
-        <v>475</v>
+        <v>425.35</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="41" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="B13" s="42">
-        <v>1998.79</v>
+        <v>5335.8</v>
       </c>
       <c r="C13" s="42"/>
       <c r="D13" s="43"/>
       <c r="E13" s="43"/>
       <c r="F13" s="44">
-        <f t="shared" si="0"/>
-        <v>1998.79</v>
+        <f>B13+C13-D13-E13</f>
+        <v>5335.8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="41" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="B14" s="42">
-        <v>425.35</v>
+        <v>475</v>
       </c>
       <c r="C14" s="42"/>
       <c r="D14" s="43"/>
       <c r="E14" s="43"/>
       <c r="F14" s="44">
         <f>B14+C14-D14-E14</f>
-        <v>425.35</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -3425,199 +3425,199 @@
         <v>94</v>
       </c>
       <c r="B15" s="42">
-        <v>1604.4</v>
+        <v>1998.79</v>
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
       <c r="F15" s="44">
         <f t="shared" si="0"/>
-        <v>1604.4</v>
+        <v>1998.79</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="41" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="B16" s="42">
-        <v>767.89999999999986</v>
+        <v>1604.4</v>
       </c>
       <c r="C16" s="42"/>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
       <c r="F16" s="44">
         <f t="shared" si="0"/>
-        <v>767.89999999999986</v>
+        <v>1604.4</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="41" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="B17" s="42">
-        <v>549.02</v>
+        <v>767.89999999999986</v>
       </c>
       <c r="C17" s="42"/>
       <c r="D17" s="43"/>
       <c r="E17" s="43"/>
       <c r="F17" s="44">
         <f t="shared" si="0"/>
-        <v>549.02</v>
+        <v>767.89999999999986</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="41" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B18" s="42">
-        <v>115.92</v>
+        <v>549.02</v>
       </c>
       <c r="C18" s="42"/>
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
       <c r="F18" s="44">
         <f t="shared" si="0"/>
-        <v>115.92</v>
+        <v>549.02</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="41" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="B19" s="42">
-        <v>3460.9099999999989</v>
+        <v>115.92</v>
       </c>
       <c r="C19" s="42"/>
       <c r="D19" s="43"/>
       <c r="E19" s="43"/>
       <c r="F19" s="44">
         <f t="shared" si="0"/>
-        <v>3460.9099999999989</v>
+        <v>115.92</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="41" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="B20" s="42">
-        <v>158.68</v>
+        <v>0</v>
       </c>
       <c r="C20" s="42"/>
       <c r="D20" s="43"/>
       <c r="E20" s="43"/>
       <c r="F20" s="44">
         <f t="shared" si="0"/>
-        <v>158.68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="41" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B21" s="42">
-        <v>998.34000000000015</v>
+        <v>3460.9099999999989</v>
       </c>
       <c r="C21" s="42"/>
       <c r="D21" s="43"/>
       <c r="E21" s="43"/>
       <c r="F21" s="44">
         <f t="shared" si="0"/>
-        <v>998.34000000000015</v>
+        <v>3460.9099999999989</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="41" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="B22" s="42">
-        <v>1060.3599999999983</v>
+        <v>158.68</v>
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="43"/>
       <c r="E22" s="43"/>
       <c r="F22" s="44">
         <f t="shared" si="0"/>
-        <v>1060.3599999999983</v>
+        <v>158.68</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="41" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B23" s="42">
-        <v>1985.5700000000006</v>
+        <v>998.34000000000015</v>
       </c>
       <c r="C23" s="42"/>
       <c r="D23" s="43"/>
       <c r="E23" s="43"/>
       <c r="F23" s="44">
         <f t="shared" si="0"/>
-        <v>1985.5700000000006</v>
+        <v>998.34000000000015</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B24" s="42">
-        <v>98.619999999999095</v>
+        <v>1060.3599999999983</v>
       </c>
       <c r="C24" s="42"/>
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
       <c r="F24" s="44">
         <f t="shared" si="0"/>
-        <v>98.619999999999095</v>
+        <v>1060.3599999999983</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="41" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="B25" s="42">
-        <v>741.9</v>
+        <v>1985.5700000000006</v>
       </c>
       <c r="C25" s="42"/>
       <c r="D25" s="43"/>
       <c r="E25" s="43"/>
       <c r="F25" s="44">
         <f t="shared" si="0"/>
-        <v>741.9</v>
+        <v>1985.5700000000006</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="B26" s="42">
-        <v>69.400000000000006</v>
+        <v>98.619999999999095</v>
       </c>
       <c r="C26" s="42"/>
       <c r="D26" s="43"/>
       <c r="E26" s="43"/>
       <c r="F26" s="44">
         <f t="shared" si="0"/>
-        <v>69.400000000000006</v>
+        <v>98.619999999999095</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="41" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B27" s="42">
-        <v>5335.8</v>
+        <v>69.400000000000006</v>
       </c>
       <c r="C27" s="42"/>
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
       <c r="F27" s="44">
-        <f>B27+C27-D27-E27</f>
-        <v>5335.8</v>
+        <f t="shared" si="0"/>
+        <v>69.400000000000006</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="41" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B28" s="42">
         <v>-459.5300000000002</v>
@@ -3632,7 +3632,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="41" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B29" s="42">
         <v>47.51</v>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="41" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B30" s="42">
         <v>2625.8999999999996</v>
@@ -3662,7 +3662,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="41" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B31" s="42">
         <v>2738.7099999999996</v>
@@ -3707,7 +3707,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="41" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B34" s="42">
         <v>0</v>
@@ -3722,7 +3722,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="41" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B35" s="42">
         <v>1269.44</v>
@@ -3737,7 +3737,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="41" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B36" s="42">
         <v>3159.3900000000003</v>
@@ -3752,22 +3752,22 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="41" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B37" s="42">
-        <v>2985.79</v>
+        <v>3727.69</v>
       </c>
       <c r="C37" s="42"/>
       <c r="D37" s="43"/>
       <c r="E37" s="43"/>
       <c r="F37" s="44">
         <f t="shared" si="0"/>
-        <v>2985.79</v>
+        <v>3727.69</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="41" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B38" s="42">
         <v>647.11</v>
@@ -3812,7 +3812,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B41" s="42">
         <v>147.06999999999994</v>
@@ -3827,7 +3827,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B42" s="42">
         <v>258.8</v>
@@ -3897,5 +3897,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>